<commit_message>
Documents: Project vision, Project Plan v1.1, Time Sheets (up to 3/11, Links)
</commit_message>
<xml_diff>
--- a/database/temp/9finder-data.xlsx
+++ b/database/temp/9finder-data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvqha_000\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1312179_Nam 4\HKI - QLDAPM\doan_nhom9\source\9Finder\database\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" tabRatio="865"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="2430" tabRatio="865"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -8965,6 +8965,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>,</t>
     </r>
@@ -8993,6 +8994,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>,</t>
     </r>

</xml_diff>